<commit_message>
Ammo text fixes and slight rebalances + RU translation
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groki\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.richard\github\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t>ammo_magnum_300</t>
   </si>
@@ -202,6 +202,21 @@
   </si>
   <si>
     <t>ammo_12x76_zhekan</t>
+  </si>
+  <si>
+    <t>ammo_23x75_shrapnel</t>
+  </si>
+  <si>
+    <t>ammo_23x75_barrikada</t>
+  </si>
+  <si>
+    <t>ammo_20x70_buck</t>
+  </si>
+  <si>
+    <t>ammo_338_federal</t>
+  </si>
+  <si>
+    <t>ammo_12x70_buck</t>
   </si>
 </sst>
 </file>
@@ -209,8 +224,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -274,13 +289,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +702,7 @@
         <v>925</v>
       </c>
       <c r="N2" s="1">
-        <f t="shared" ref="N2:N26" si="0">LOG10(1/M2*1000)*2</f>
+        <f t="shared" ref="N2:N24" si="0">LOG10(1/M2*1000)*2</f>
         <v>6.7716534521934837E-2</v>
       </c>
       <c r="O2">
@@ -704,91 +719,72 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>6600</v>
+      </c>
+      <c r="D3" s="4">
+        <f>C3/10</f>
+        <v>660</v>
+      </c>
+      <c r="E3" s="9">
+        <f>K3/D3</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="F3" s="8">
+        <f>G3/D3*100</f>
+        <v>0.11363636363636363</v>
+      </c>
+      <c r="G3">
+        <v>0.75</v>
+      </c>
+      <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3">
-        <v>2035</v>
-      </c>
-      <c r="D3" s="4">
-        <f>C3/15</f>
-        <v>135.66666666666666</v>
-      </c>
-      <c r="E3" s="9">
-        <f t="shared" ref="E2:E26" si="1">K3/D3</f>
-        <v>0.57721621621621622</v>
-      </c>
-      <c r="F3" s="9">
-        <f t="shared" ref="F3:F36" si="2">G3/D3*100</f>
-        <v>0.18427518427518427</v>
-      </c>
-      <c r="G3">
-        <v>0.25</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1.1299999999999999</v>
-      </c>
       <c r="I3">
-        <v>1.05</v>
+        <v>0.85</v>
       </c>
       <c r="J3">
-        <f>I3*H3</f>
-        <v>1.1864999999999999</v>
+        <f>H3*I3</f>
+        <v>0.85</v>
       </c>
       <c r="K3" s="2">
         <f>J3*Feuil2!$B$1</f>
-        <v>78.308999999999997</v>
-      </c>
-      <c r="L3" s="1">
-        <v>4064</v>
-      </c>
-      <c r="M3" s="1">
-        <v>820</v>
-      </c>
-      <c r="N3" s="1">
-        <f t="shared" si="0"/>
-        <v>0.17237229523256661</v>
-      </c>
-      <c r="O3">
-        <f>L3/Feuil2!$B$2</f>
-        <v>1.1409320606400899</v>
-      </c>
-      <c r="P3">
-        <f>O3*Feuil2!$B$3</f>
-        <v>80.196114542391911</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q22" si="3">P3*N3+P3</f>
-        <v>94.019702874797815</v>
-      </c>
+        <v>56.1</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>54</v>
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
       </c>
       <c r="C4">
-        <v>7000</v>
+        <v>2035</v>
       </c>
       <c r="D4" s="4">
         <f>C4/15</f>
-        <v>466.66666666666669</v>
+        <v>135.66666666666666</v>
       </c>
       <c r="E4" s="9">
-        <f t="shared" si="1"/>
-        <v>0.16780499999999998</v>
-      </c>
-      <c r="F4" s="8">
-        <f t="shared" si="2"/>
-        <v>8.357142857142856E-2</v>
+        <f t="shared" ref="E4:E27" si="1">K4/D4</f>
+        <v>0.57721621621621622</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" ref="F4:F37" si="2">G4/D4*100</f>
+        <v>0.18427518427518427</v>
       </c>
       <c r="G4">
-        <v>0.39</v>
+        <v>0.25</v>
       </c>
       <c r="H4" s="3">
         <v>1.1299999999999999</v>
@@ -823,96 +819,96 @@
         <v>80.196114542391911</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4" si="4">P4*N4+P4</f>
+        <f t="shared" ref="Q4:Q23" si="3">P4*N4+P4</f>
         <v>94.019702874797815</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
+      <c r="A5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C5">
-        <v>2800</v>
+        <v>7000</v>
       </c>
       <c r="D5" s="4">
-        <f>C5/10</f>
-        <v>280</v>
+        <f>C5/15</f>
+        <v>466.66666666666669</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" si="1"/>
-        <v>0.26369357142857142</v>
-      </c>
-      <c r="F5" s="9">
-        <f t="shared" si="2"/>
-        <v>0.11071428571428571</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.31</v>
+        <v>0.16780499999999998</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="2"/>
+        <v>8.357142857142856E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.39</v>
       </c>
       <c r="H5" s="3">
-        <v>1.0169999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="I5">
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J18" si="5">I5*H5</f>
-        <v>1.1187</v>
+        <f>I5*H5</f>
+        <v>1.1864999999999999</v>
       </c>
       <c r="K5" s="2">
         <f>J5*Feuil2!$B$1</f>
-        <v>73.834199999999996</v>
+        <v>78.308999999999997</v>
       </c>
       <c r="L5" s="1">
-        <v>3744</v>
+        <v>4064</v>
       </c>
       <c r="M5" s="1">
-        <v>800</v>
+        <v>820</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="0"/>
-        <v>0.19382002601611284</v>
+        <v>0.17237229523256661</v>
       </c>
       <c r="O5">
         <f>L5/Feuil2!$B$2</f>
-        <v>1.051094890510949</v>
+        <v>1.1409320606400899</v>
       </c>
       <c r="P5">
         <f>O5*Feuil2!$B$3</f>
-        <v>73.881459854014594</v>
+        <v>80.196114542391911</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="3"/>
-        <v>88.201166325028098</v>
+        <f t="shared" ref="Q5" si="4">P5*N5+P5</f>
+        <v>94.019702874797815</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>54</v>
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
       </c>
       <c r="C6">
-        <v>10150</v>
+        <v>2800</v>
       </c>
       <c r="D6" s="4">
         <f>C6/10</f>
-        <v>1015</v>
+        <v>280</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" si="1"/>
-        <v>7.274305418719211E-2</v>
-      </c>
-      <c r="F6" s="8">
-        <f t="shared" si="2"/>
-        <v>7.8817733990147784E-2</v>
+        <v>0.26369357142857142</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="2"/>
+        <v>0.11071428571428571</v>
       </c>
       <c r="G6" s="3">
-        <v>0.8</v>
+        <v>0.31</v>
       </c>
       <c r="H6" s="3">
         <v>1.0169999999999999</v>
@@ -921,7 +917,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J6">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="J6:J19" si="5">I6*H6</f>
         <v>1.1187</v>
       </c>
       <c r="K6" s="2">
@@ -952,29 +948,29 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
+      <c r="A7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C7">
-        <v>4000</v>
+        <v>10150</v>
       </c>
       <c r="D7" s="4">
         <f>C7/10</f>
-        <v>400</v>
+        <v>1015</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="1"/>
-        <v>0.18458549999999999</v>
-      </c>
-      <c r="F7" s="9">
-        <f t="shared" si="2"/>
-        <v>0.11250000000000002</v>
+        <v>7.274305418719211E-2</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="2"/>
+        <v>7.8817733990147784E-2</v>
       </c>
       <c r="G7" s="3">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="H7" s="3">
         <v>1.0169999999999999</v>
@@ -1015,90 +1011,90 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>56</v>
       </c>
       <c r="C8">
-        <v>2250</v>
+        <v>4000</v>
       </c>
       <c r="D8" s="4">
-        <f>C8/15</f>
-        <v>150</v>
+        <f>C8/10</f>
+        <v>400</v>
       </c>
       <c r="E8" s="9">
         <f t="shared" si="1"/>
-        <v>0.46859999999999996</v>
+        <v>0.18458549999999999</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="2"/>
-        <v>0.22666666666666668</v>
+        <v>0.11250000000000002</v>
       </c>
       <c r="G8" s="3">
-        <v>0.34</v>
+        <v>0.45</v>
       </c>
       <c r="H8" s="3">
-        <v>1.0649999999999999</v>
+        <v>1.0169999999999999</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J8">
         <f t="shared" si="5"/>
-        <v>1.0649999999999999</v>
+        <v>1.1187</v>
       </c>
       <c r="K8" s="2">
         <f>J8*Feuil2!$B$1</f>
-        <v>70.289999999999992</v>
+        <v>73.834199999999996</v>
       </c>
       <c r="L8" s="1">
-        <v>3562</v>
+        <v>3744</v>
       </c>
       <c r="M8" s="1">
-        <v>790</v>
+        <v>800</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
-        <v>0.20474581741911721</v>
+        <v>0.19382002601611284</v>
       </c>
       <c r="O8">
         <f>L8/Feuil2!$B$2</f>
-        <v>1</v>
+        <v>1.051094890510949</v>
       </c>
       <c r="P8">
         <f>O8*Feuil2!$B$3</f>
-        <v>70.289999999999992</v>
+        <v>73.881459854014594</v>
       </c>
       <c r="Q8">
         <f t="shared" si="3"/>
-        <v>84.681583506389742</v>
+        <v>88.201166325028098</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>54</v>
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
       </c>
       <c r="C9">
-        <v>7500</v>
+        <v>2250</v>
       </c>
       <c r="D9" s="4">
         <f>C9/15</f>
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="E9" s="9">
         <f t="shared" si="1"/>
-        <v>0.14057999999999998</v>
-      </c>
-      <c r="F9" s="8">
-        <f t="shared" si="2"/>
-        <v>0.124</v>
+        <v>0.46859999999999996</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="2"/>
+        <v>0.22666666666666668</v>
       </c>
       <c r="G9" s="3">
-        <v>0.62</v>
+        <v>0.34</v>
       </c>
       <c r="H9" s="3">
         <v>1.0649999999999999</v>
@@ -1138,91 +1134,91 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>56</v>
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C10">
-        <v>3200</v>
+        <v>7500</v>
       </c>
       <c r="D10" s="4">
-        <f>C10/10</f>
-        <v>320</v>
+        <f>C10/15</f>
+        <v>500</v>
       </c>
       <c r="E10" s="9">
         <f t="shared" si="1"/>
-        <v>0.25059375000000006</v>
-      </c>
-      <c r="F10" s="9">
-        <f t="shared" si="2"/>
-        <v>0.11874999999999999</v>
+        <v>0.14057999999999998</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="2"/>
+        <v>0.124</v>
       </c>
       <c r="G10" s="3">
-        <v>0.38</v>
+        <v>0.62</v>
       </c>
       <c r="H10" s="3">
-        <v>1.35</v>
+        <v>1.0649999999999999</v>
       </c>
       <c r="I10">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <f t="shared" si="5"/>
-        <v>1.2150000000000001</v>
+        <v>1.0649999999999999</v>
       </c>
       <c r="K10" s="2">
         <f>J10*Feuil2!$B$1</f>
-        <v>80.190000000000012</v>
+        <v>70.289999999999992</v>
       </c>
       <c r="L10" s="1">
-        <v>3307</v>
+        <v>3562</v>
       </c>
       <c r="M10" s="1">
-        <v>295</v>
+        <v>790</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
-        <v>1.060355968043674</v>
+        <v>0.20474581741911721</v>
       </c>
       <c r="O10">
         <f>L10/Feuil2!$B$2</f>
-        <v>0.92841100505334084</v>
+        <v>1</v>
       </c>
       <c r="P10">
         <f>O10*Feuil2!$B$3</f>
-        <v>65.258009545199315</v>
+        <v>70.289999999999992</v>
       </c>
       <c r="Q10">
         <f t="shared" si="3"/>
-        <v>134.45472942910246</v>
+        <v>84.681583506389742</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>54</v>
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
       </c>
       <c r="C11">
-        <v>7500</v>
+        <v>3200</v>
       </c>
       <c r="D11" s="4">
         <f>C11/10</f>
-        <v>750</v>
+        <v>320</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" si="1"/>
-        <v>0.10692000000000002</v>
-      </c>
-      <c r="F11" s="8">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.25059375000000006</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="2"/>
+        <v>0.11874999999999999</v>
       </c>
       <c r="G11" s="3">
-        <v>0.75</v>
+        <v>0.38</v>
       </c>
       <c r="H11" s="3">
         <v>1.35</v>
@@ -1245,7 +1241,7 @@
         <v>295</v>
       </c>
       <c r="N11" s="1">
-        <f>LOG10(1/M11*1000)*2</f>
+        <f t="shared" si="0"/>
         <v>1.060355968043674</v>
       </c>
       <c r="O11">
@@ -1257,110 +1253,110 @@
         <v>65.258009545199315</v>
       </c>
       <c r="Q11">
-        <f>P11*N11+P11</f>
+        <f t="shared" si="3"/>
         <v>134.45472942910246</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1350</v>
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12">
+        <v>7500</v>
       </c>
       <c r="D12" s="4">
-        <f>C12/15</f>
-        <v>90</v>
+        <f>C12/10</f>
+        <v>750</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>0.40333333333333338</v>
-      </c>
-      <c r="F12" s="9">
-        <f t="shared" si="2"/>
-        <v>0.27777777777777779</v>
+        <v>0.10692000000000002</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="G12" s="3">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="H12" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.35</v>
       </c>
       <c r="I12">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="J12">
         <f t="shared" si="5"/>
-        <v>0.55000000000000004</v>
+        <v>1.2150000000000001</v>
       </c>
       <c r="K12" s="2">
         <f>J12*Feuil2!$B$1</f>
-        <v>36.300000000000004</v>
+        <v>80.190000000000012</v>
       </c>
       <c r="L12" s="1">
-        <v>1461</v>
+        <v>3307</v>
       </c>
       <c r="M12" s="1">
-        <v>880</v>
+        <v>295</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.11103465569966266</v>
+        <f>LOG10(1/M12*1000)*2</f>
+        <v>1.060355968043674</v>
       </c>
       <c r="O12">
         <f>L12/Feuil2!$B$2</f>
-        <v>0.41016282987085906</v>
+        <v>0.92841100505334084</v>
       </c>
       <c r="P12">
         <f>O12*Feuil2!$B$3</f>
-        <v>28.830345311622679</v>
+        <v>65.258009545199315</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="3"/>
-        <v>32.031512777001083</v>
+        <f>P12*N12+P12</f>
+        <v>134.45472942910246</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>55</v>
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
       </c>
       <c r="C13" s="3">
-        <v>2000</v>
+        <v>1350</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" ref="D13:D21" si="6">C13/15</f>
-        <v>133.33333333333334</v>
-      </c>
-      <c r="E13" s="10">
+        <f>C13/15</f>
+        <v>90</v>
+      </c>
+      <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>0.39600000000000002</v>
+        <v>0.40333333333333338</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="2"/>
-        <v>0.11249999999999999</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="G13" s="3">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="H13" s="3">
-        <v>1.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I13">
         <v>0.5</v>
       </c>
       <c r="J13">
-        <f t="shared" ref="J13:J14" si="7">I13*H13</f>
-        <v>0.8</v>
+        <f t="shared" si="5"/>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K13" s="2">
         <f>J13*Feuil2!$B$1</f>
-        <v>52.800000000000004</v>
+        <v>36.300000000000004</v>
       </c>
       <c r="L13" s="1">
         <v>1461</v>
@@ -1386,43 +1382,43 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>54</v>
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C14" s="3">
-        <v>5100</v>
+        <v>2000</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="6"/>
-        <v>340</v>
-      </c>
-      <c r="E14" s="9">
+        <f t="shared" ref="D14:D22" si="6">C14/15</f>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="E14" s="10">
         <f t="shared" si="1"/>
-        <v>0.10676470588235296</v>
-      </c>
-      <c r="F14" s="8">
-        <f t="shared" si="2"/>
-        <v>0.13823529411764704</v>
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F14" s="9">
+        <f t="shared" si="2"/>
+        <v>0.11249999999999999</v>
       </c>
       <c r="G14" s="3">
-        <v>0.47</v>
+        <v>0.15</v>
       </c>
       <c r="H14" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="I14">
         <v>0.5</v>
       </c>
       <c r="J14">
-        <f t="shared" si="7"/>
-        <v>0.55000000000000004</v>
+        <f t="shared" ref="J14:J15" si="7">I14*H14</f>
+        <v>0.8</v>
       </c>
       <c r="K14" s="2">
         <f>J14*Feuil2!$B$1</f>
-        <v>36.300000000000004</v>
+        <v>52.800000000000004</v>
       </c>
       <c r="L14" s="1">
         <v>1461</v>
@@ -1448,105 +1444,105 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
+      <c r="A15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C15" s="3">
-        <v>1500</v>
+        <v>5100</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="6"/>
-        <v>100</v>
+        <v>340</v>
       </c>
       <c r="E15" s="9">
         <f t="shared" si="1"/>
-        <v>0.34649999999999997</v>
-      </c>
-      <c r="F15" s="9">
-        <f t="shared" si="2"/>
-        <v>0.27</v>
+        <v>0.10676470588235296</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="2"/>
+        <v>0.13823529411764704</v>
       </c>
       <c r="G15" s="3">
-        <v>0.27</v>
+        <v>0.47</v>
       </c>
       <c r="H15" s="3">
-        <v>1.05</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I15">
         <v>0.5</v>
       </c>
       <c r="J15">
+        <f t="shared" si="7"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K15" s="2">
+        <f>J15*Feuil2!$B$1</f>
+        <v>36.300000000000004</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1461</v>
+      </c>
+      <c r="M15" s="1">
+        <v>880</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.11103465569966266</v>
+      </c>
+      <c r="O15">
+        <f>L15/Feuil2!$B$2</f>
+        <v>0.41016282987085906</v>
+      </c>
+      <c r="P15">
+        <f>O15*Feuil2!$B$3</f>
+        <v>28.830345311622679</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="3"/>
+        <v>32.031512777001083</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1500</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="E16" s="9">
+        <f t="shared" si="1"/>
+        <v>0.34649999999999997</v>
+      </c>
+      <c r="F16" s="9">
+        <f t="shared" si="2"/>
+        <v>0.27</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1.05</v>
+      </c>
+      <c r="I16">
+        <v>0.5</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="5"/>
         <v>0.52500000000000002</v>
       </c>
-      <c r="K15" s="2">
-        <f>J15*Feuil2!$B$1</f>
-        <v>34.65</v>
-      </c>
-      <c r="L15" s="1">
-        <v>1859</v>
-      </c>
-      <c r="M15" s="1">
-        <v>948</v>
-      </c>
-      <c r="N15" s="1">
-        <f t="shared" si="0"/>
-        <v>4.6383325323867484E-2</v>
-      </c>
-      <c r="O15">
-        <f>L15/Feuil2!$B$2</f>
-        <v>0.52189781021897808</v>
-      </c>
-      <c r="P15">
-        <f>O15*Feuil2!$B$3</f>
-        <v>36.684197080291966</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="3"/>
-        <v>38.385732127712018</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1850</v>
-      </c>
-      <c r="D16" s="4">
-        <f t="shared" si="6"/>
-        <v>123.33333333333333</v>
-      </c>
-      <c r="E16" s="10">
-        <f t="shared" si="1"/>
-        <v>0.3745945945945946</v>
-      </c>
-      <c r="F16" s="9">
-        <f t="shared" si="2"/>
-        <v>0.12162162162162161</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="H16" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="I16">
-        <v>0.5</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="5"/>
-        <v>0.7</v>
-      </c>
       <c r="K16" s="2">
         <f>J16*Feuil2!$B$1</f>
-        <v>46.199999999999996</v>
+        <v>34.65</v>
       </c>
       <c r="L16" s="1">
         <v>1859</v>
@@ -1572,43 +1568,43 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>54</v>
+      <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C17" s="3">
-        <v>5500</v>
+        <v>1850</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="6"/>
-        <v>366.66666666666669</v>
-      </c>
-      <c r="E17" s="9">
+        <v>123.33333333333333</v>
+      </c>
+      <c r="E17" s="10">
         <f t="shared" si="1"/>
-        <v>9.4499999999999987E-2</v>
-      </c>
-      <c r="F17" s="8">
-        <f t="shared" si="2"/>
-        <v>0.14181818181818182</v>
+        <v>0.3745945945945946</v>
+      </c>
+      <c r="F17" s="9">
+        <f t="shared" si="2"/>
+        <v>0.12162162162162161</v>
       </c>
       <c r="G17" s="3">
-        <v>0.52</v>
+        <v>0.15</v>
       </c>
       <c r="H17" s="3">
-        <v>1.05</v>
+        <v>1.4</v>
       </c>
       <c r="I17">
         <v>0.5</v>
       </c>
       <c r="J17">
-        <f t="shared" ref="J17" si="8">I17*H17</f>
-        <v>0.52500000000000002</v>
+        <f t="shared" si="5"/>
+        <v>0.7</v>
       </c>
       <c r="K17" s="2">
         <f>J17*Feuil2!$B$1</f>
-        <v>34.65</v>
+        <v>46.199999999999996</v>
       </c>
       <c r="L17" s="1">
         <v>1859</v>
@@ -1634,91 +1630,91 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>56</v>
+      <c r="A18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C18" s="3">
-        <v>1950</v>
+        <v>5500</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="6"/>
-        <v>130</v>
+        <v>366.66666666666669</v>
       </c>
       <c r="E18" s="9">
         <f t="shared" si="1"/>
-        <v>0.30918461538461539</v>
-      </c>
-      <c r="F18" s="9">
-        <f t="shared" si="2"/>
-        <v>0.23076923076923075</v>
+        <v>9.4499999999999987E-2</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="2"/>
+        <v>0.14181818181818182</v>
       </c>
       <c r="G18" s="3">
-        <v>0.3</v>
+        <v>0.52</v>
       </c>
       <c r="H18" s="3">
         <v>1.05</v>
       </c>
       <c r="I18">
-        <v>0.57999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="J18">
-        <f t="shared" si="5"/>
-        <v>0.60899999999999999</v>
+        <f t="shared" ref="J18" si="8">I18*H18</f>
+        <v>0.52500000000000002</v>
       </c>
       <c r="K18" s="2">
         <f>J18*Feuil2!$B$1</f>
-        <v>40.194000000000003</v>
+        <v>34.65</v>
       </c>
       <c r="L18" s="1">
-        <v>2179</v>
+        <v>1859</v>
       </c>
       <c r="M18" s="1">
-        <v>738</v>
+        <v>948</v>
       </c>
       <c r="N18" s="1">
         <f t="shared" si="0"/>
-        <v>0.2638872763539169</v>
+        <v>4.6383325323867484E-2</v>
       </c>
       <c r="O18">
         <f>L18/Feuil2!$B$2</f>
-        <v>0.61173498034811902</v>
+        <v>0.52189781021897808</v>
       </c>
       <c r="P18">
         <f>O18*Feuil2!$B$3</f>
-        <v>42.998851768669283</v>
+        <v>36.684197080291966</v>
       </c>
       <c r="Q18">
         <f t="shared" si="3"/>
-        <v>54.345701648249225</v>
+        <v>38.385732127712018</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>54</v>
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
       </c>
       <c r="C19" s="3">
-        <v>5900</v>
+        <v>1950</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="6"/>
-        <v>393.33333333333331</v>
+        <v>130</v>
       </c>
       <c r="E19" s="9">
         <f t="shared" si="1"/>
-        <v>0.10218813559322035</v>
+        <v>0.30918461538461539</v>
       </c>
       <c r="F19" s="9">
         <f t="shared" si="2"/>
-        <v>0.13983050847457629</v>
+        <v>0.23076923076923075</v>
       </c>
       <c r="G19" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="H19" s="3">
         <v>1.05</v>
@@ -1727,7 +1723,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="J19">
-        <f t="shared" ref="J19:J20" si="9">I19*H19</f>
+        <f t="shared" si="5"/>
         <v>0.60899999999999999</v>
       </c>
       <c r="K19" s="2">
@@ -1758,91 +1754,91 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>56</v>
+      <c r="A20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C20" s="3">
-        <v>1600</v>
+        <v>5900</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="6"/>
-        <v>106.66666666666667</v>
+        <v>393.33333333333331</v>
       </c>
       <c r="E20" s="9">
         <f t="shared" si="1"/>
-        <v>0.36444374999999996</v>
+        <v>0.10218813559322035</v>
       </c>
       <c r="F20" s="9">
         <f t="shared" si="2"/>
-        <v>0.28125</v>
+        <v>0.13983050847457629</v>
       </c>
       <c r="G20" s="3">
-        <v>0.3</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H20" s="3">
-        <v>0.95</v>
+        <v>1.05</v>
       </c>
       <c r="I20">
-        <v>0.62</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J20">
-        <f t="shared" si="9"/>
-        <v>0.58899999999999997</v>
+        <f t="shared" ref="J20:J21" si="9">I20*H20</f>
+        <v>0.60899999999999999</v>
       </c>
       <c r="K20" s="2">
         <f>J20*Feuil2!$B$1</f>
-        <v>38.873999999999995</v>
+        <v>40.194000000000003</v>
       </c>
       <c r="L20" s="1">
-        <v>964</v>
+        <v>2179</v>
       </c>
       <c r="M20" s="1">
-        <v>327</v>
+        <v>738</v>
       </c>
       <c r="N20" s="1">
         <f t="shared" si="0"/>
-        <v>0.97090449467942785</v>
+        <v>0.2638872763539169</v>
       </c>
       <c r="O20">
         <f>L20/Feuil2!$B$2</f>
-        <v>0.27063447501403703</v>
+        <v>0.61173498034811902</v>
       </c>
       <c r="P20">
         <f>O20*Feuil2!$B$3</f>
-        <v>19.022897248736662</v>
+        <v>42.998851768669283</v>
       </c>
       <c r="Q20">
         <f t="shared" si="3"/>
-        <v>37.49231368936001</v>
+        <v>54.345701648249225</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>54</v>
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>56</v>
       </c>
       <c r="C21" s="3">
-        <v>5200</v>
+        <v>1600</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="6"/>
-        <v>346.66666666666669</v>
+        <v>106.66666666666667</v>
       </c>
       <c r="E21" s="9">
         <f t="shared" si="1"/>
-        <v>0.11213653846153844</v>
-      </c>
-      <c r="F21" s="8">
-        <f t="shared" si="2"/>
-        <v>0.1528846153846154</v>
+        <v>0.36444374999999996</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="2"/>
+        <v>0.28125</v>
       </c>
       <c r="G21" s="3">
-        <v>0.53</v>
+        <v>0.3</v>
       </c>
       <c r="H21" s="3">
         <v>0.95</v>
@@ -1851,7 +1847,7 @@
         <v>0.62</v>
       </c>
       <c r="J21">
-        <f t="shared" ref="J21" si="10">I21*H21</f>
+        <f t="shared" si="9"/>
         <v>0.58899999999999997</v>
       </c>
       <c r="K21" s="2">
@@ -1877,173 +1873,173 @@
         <v>19.022897248736662</v>
       </c>
       <c r="Q21">
-        <f t="shared" ref="Q21" si="11">P21*N21+P21</f>
+        <f t="shared" si="3"/>
         <v>37.49231368936001</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="3">
+        <v>5200</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="6"/>
+        <v>346.66666666666669</v>
+      </c>
+      <c r="E22" s="9">
+        <f t="shared" si="1"/>
+        <v>0.11213653846153844</v>
+      </c>
+      <c r="F22" s="8">
+        <f t="shared" si="2"/>
+        <v>0.1528846153846154</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I22">
+        <v>0.62</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22" si="10">I22*H22</f>
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="K22" s="2">
+        <f>J22*Feuil2!$B$1</f>
+        <v>38.873999999999995</v>
+      </c>
+      <c r="L22" s="1">
+        <v>964</v>
+      </c>
+      <c r="M22" s="1">
+        <v>327</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.97090449467942785</v>
+      </c>
+      <c r="O22">
+        <f>L22/Feuil2!$B$2</f>
+        <v>0.27063447501403703</v>
+      </c>
+      <c r="P22">
+        <f>O22*Feuil2!$B$3</f>
+        <v>19.022897248736662</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" ref="Q22" si="11">P22*N22+P22</f>
+        <v>37.49231368936001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C23" s="3">
         <v>2600</v>
       </c>
-      <c r="D22" s="4">
-        <f>C22/13</f>
+      <c r="D23" s="4">
+        <f>C23/13</f>
         <v>200</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E23" s="10">
         <f t="shared" si="1"/>
         <v>0.47519999999999996</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F23" s="9">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G23" s="3">
         <v>0.3</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H23" s="3">
         <f>1.2*2</f>
         <v>2.4</v>
       </c>
-      <c r="I22">
+      <c r="I23">
         <v>0.6</v>
       </c>
-      <c r="J22">
-        <f t="shared" ref="J22:J23" si="12">I22*H22</f>
+      <c r="J23">
+        <f t="shared" ref="J23:J24" si="12">I23*H23</f>
         <v>1.44</v>
       </c>
-      <c r="K22" s="2">
-        <f>J22*Feuil2!$B$1</f>
+      <c r="K23" s="2">
+        <f>J23*Feuil2!$B$1</f>
         <v>95.039999999999992</v>
       </c>
-      <c r="L22" s="1">
+      <c r="L23" s="1">
         <v>1062</v>
       </c>
-      <c r="M22" s="1">
+      <c r="M23" s="1">
         <v>430</v>
       </c>
-      <c r="N22" s="1">
+      <c r="N23" s="1">
         <f t="shared" si="0"/>
         <v>0.73306308884082705</v>
       </c>
-      <c r="O22">
-        <f>L22/Feuil2!$B$2</f>
+      <c r="O23">
+        <f>L23/Feuil2!$B$2</f>
         <v>0.29814710836608649</v>
       </c>
-      <c r="P22">
-        <f>O22*Feuil2!$B$3</f>
+      <c r="P23">
+        <f>O23*Feuil2!$B$3</f>
         <v>20.956760247052216</v>
       </c>
-      <c r="Q22">
+      <c r="Q23">
         <f t="shared" si="3"/>
         <v>36.31938764585297</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C24" s="3">
         <v>560</v>
       </c>
-      <c r="D23" s="4">
-        <f>C23/15</f>
+      <c r="D24" s="4">
+        <f>C24/15</f>
         <v>37.333333333333336</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E24" s="9">
         <f t="shared" si="1"/>
         <v>0.47732142857142856</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F24" s="9">
         <f t="shared" si="2"/>
         <v>0.40178571428571425</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G24" s="3">
         <v>0.15</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H24" s="3">
         <v>0.6</v>
       </c>
-      <c r="I23">
+      <c r="I24">
         <v>0.45</v>
       </c>
-      <c r="J23">
+      <c r="J24">
         <f t="shared" si="12"/>
         <v>0.27</v>
       </c>
-      <c r="K23" s="2">
-        <f>J23*Feuil2!$B$1</f>
-        <v>17.82</v>
-      </c>
-      <c r="L23" s="1">
-        <v>378</v>
-      </c>
-      <c r="M23" s="1">
-        <v>351</v>
-      </c>
-      <c r="N23" s="1">
-        <f t="shared" si="0"/>
-        <v>0.90938576706835184</v>
-      </c>
-      <c r="O23">
-        <f>L23/Feuil2!$B$2</f>
-        <v>0.10612015721504772</v>
-      </c>
-      <c r="P23">
-        <f>O23*Feuil2!$B$3</f>
-        <v>7.4591858506457038</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" ref="Q23" si="13">P23*N23+P23</f>
-        <v>14.242463297140544</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="3">
-        <v>960</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" ref="D24:D31" si="14">C24/15</f>
-        <v>64</v>
-      </c>
-      <c r="E24" s="10">
-        <f t="shared" si="1"/>
-        <v>0.51046875000000003</v>
-      </c>
-      <c r="F24" s="9">
-        <f t="shared" si="2"/>
-        <v>0.15625</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H24" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I24">
-        <v>0.45</v>
-      </c>
-      <c r="J24">
-        <f t="shared" ref="J24:J26" si="15">I24*H24</f>
-        <v>0.49500000000000005</v>
-      </c>
       <c r="K24" s="2">
         <f>J24*Feuil2!$B$1</f>
-        <v>32.67</v>
+        <v>17.82</v>
       </c>
       <c r="L24" s="1">
         <v>378</v>
@@ -2052,7 +2048,7 @@
         <v>351</v>
       </c>
       <c r="N24" s="1">
-        <f>LOG10(1/M24*1000)*2</f>
+        <f t="shared" si="0"/>
         <v>0.90938576706835184</v>
       </c>
       <c r="O24">
@@ -2064,48 +2060,48 @@
         <v>7.4591858506457038</v>
       </c>
       <c r="Q24">
-        <f t="shared" ref="Q24:Q25" si="16">P24*N24+P24</f>
+        <f t="shared" ref="Q24" si="13">P24*N24+P24</f>
         <v>14.242463297140544</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>54</v>
+      <c r="A25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C25" s="3">
-        <v>1200</v>
+        <v>960</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="14"/>
-        <v>80</v>
-      </c>
-      <c r="E25" s="9">
+        <f t="shared" ref="D25:D32" si="14">C25/15</f>
+        <v>64</v>
+      </c>
+      <c r="E25" s="10">
         <f t="shared" si="1"/>
-        <v>0.22275</v>
-      </c>
-      <c r="F25" s="8">
-        <f t="shared" si="2"/>
-        <v>0.375</v>
+        <v>0.51046875000000003</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="2"/>
+        <v>0.15625</v>
       </c>
       <c r="G25" s="3">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H25" s="3">
-        <v>0.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I25">
         <v>0.45</v>
       </c>
       <c r="J25">
-        <f t="shared" si="15"/>
-        <v>0.27</v>
+        <f t="shared" ref="J25:J27" si="15">I25*H25</f>
+        <v>0.49500000000000005</v>
       </c>
       <c r="K25" s="2">
         <f>J25*Feuil2!$B$1</f>
-        <v>17.82</v>
+        <v>32.67</v>
       </c>
       <c r="L25" s="1">
         <v>378</v>
@@ -2114,7 +2110,7 @@
         <v>351</v>
       </c>
       <c r="N25" s="1">
-        <f>LOG10(1/M25*1000)*2</f>
+        <f t="shared" ref="N25:N32" si="16">LOG10(1/M25*1000)*2</f>
         <v>0.90938576706835184</v>
       </c>
       <c r="O25">
@@ -2126,110 +2122,110 @@
         <v>7.4591858506457038</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="Q25:Q26" si="17">P25*N25+P25</f>
         <v>14.242463297140544</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" t="s">
-        <v>56</v>
+      <c r="A26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C26" s="3">
-        <v>645</v>
+        <v>1200</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="14"/>
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="E26" s="9">
         <f t="shared" si="1"/>
-        <v>0.48348837209302326</v>
-      </c>
-      <c r="F26" s="9">
-        <f t="shared" si="2"/>
-        <v>0.39534883720930236</v>
+        <v>0.22275</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" si="2"/>
+        <v>0.375</v>
       </c>
       <c r="G26" s="3">
-        <v>0.17</v>
+        <v>0.3</v>
       </c>
       <c r="H26" s="3">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="I26">
         <v>0.45</v>
       </c>
       <c r="J26">
         <f t="shared" si="15"/>
-        <v>0.315</v>
+        <v>0.27</v>
       </c>
       <c r="K26" s="2">
         <f>J26*Feuil2!$B$1</f>
-        <v>20.79</v>
+        <v>17.82</v>
       </c>
       <c r="L26" s="1">
-        <v>675</v>
+        <v>378</v>
       </c>
       <c r="M26" s="1">
-        <v>410</v>
+        <v>351</v>
       </c>
       <c r="N26" s="1">
-        <f>LOG10(1/M26*1000)*2</f>
-        <v>0.77443228656052898</v>
+        <f t="shared" si="16"/>
+        <v>0.90938576706835184</v>
       </c>
       <c r="O26">
         <f>L26/Feuil2!$B$2</f>
-        <v>0.18950028074115666</v>
+        <v>0.10612015721504772</v>
       </c>
       <c r="P26">
         <f>O26*Feuil2!$B$3</f>
-        <v>13.319974733295901</v>
+        <v>7.4591858506457038</v>
       </c>
       <c r="Q26">
-        <f t="shared" ref="Q26" si="17">P26*N26+P26</f>
-        <v>23.635393222930716</v>
+        <f t="shared" si="17"/>
+        <v>14.242463297140544</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>55</v>
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
       </c>
       <c r="C27" s="3">
-        <v>1125</v>
+        <v>645</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="14"/>
-        <v>75</v>
-      </c>
-      <c r="E27" s="10">
-        <f>K27/D27</f>
-        <v>0.53460000000000008</v>
+        <v>43</v>
+      </c>
+      <c r="E27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.48348837209302326</v>
       </c>
       <c r="F27" s="9">
         <f t="shared" si="2"/>
-        <v>0.13333333333333336</v>
+        <v>0.39534883720930236</v>
       </c>
       <c r="G27" s="3">
-        <v>0.1</v>
+        <v>0.17</v>
       </c>
       <c r="H27" s="3">
-        <v>1.35</v>
+        <v>0.7</v>
       </c>
       <c r="I27">
         <v>0.45</v>
       </c>
       <c r="J27">
-        <f t="shared" ref="J27:J30" si="18">I27*H27</f>
-        <v>0.60750000000000004</v>
+        <f t="shared" si="15"/>
+        <v>0.315</v>
       </c>
       <c r="K27" s="2">
         <f>J27*Feuil2!$B$1</f>
-        <v>40.095000000000006</v>
+        <v>20.79</v>
       </c>
       <c r="L27" s="1">
         <v>675</v>
@@ -2238,7 +2234,7 @@
         <v>410</v>
       </c>
       <c r="N27" s="1">
-        <f>LOG10(1/M27*1000)*2</f>
+        <f t="shared" si="16"/>
         <v>0.77443228656052898</v>
       </c>
       <c r="O27">
@@ -2250,48 +2246,48 @@
         <v>13.319974733295901</v>
       </c>
       <c r="Q27">
-        <f t="shared" ref="Q27:Q28" si="19">P27*N27+P27</f>
+        <f t="shared" ref="Q27" si="18">P27*N27+P27</f>
         <v>23.635393222930716</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>54</v>
+      <c r="A28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C28" s="3">
-        <v>2350</v>
+        <v>1125</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="14"/>
-        <v>156.66666666666666</v>
-      </c>
-      <c r="E28" s="9">
-        <f t="shared" ref="E28:E36" si="20">K28/D28</f>
-        <v>0.13270212765957448</v>
-      </c>
-      <c r="F28" s="8">
-        <f t="shared" si="2"/>
-        <v>0.24255319148936172</v>
+        <v>75</v>
+      </c>
+      <c r="E28" s="10">
+        <f>K28/D28</f>
+        <v>0.53460000000000008</v>
+      </c>
+      <c r="F28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.13333333333333336</v>
       </c>
       <c r="G28" s="3">
-        <v>0.38</v>
+        <v>0.1</v>
       </c>
       <c r="H28" s="3">
-        <v>0.7</v>
+        <v>1.35</v>
       </c>
       <c r="I28">
         <v>0.45</v>
       </c>
       <c r="J28">
-        <f t="shared" si="18"/>
-        <v>0.315</v>
+        <f t="shared" ref="J28:J31" si="19">I28*H28</f>
+        <v>0.60750000000000004</v>
       </c>
       <c r="K28" s="2">
         <f>J28*Feuil2!$B$1</f>
-        <v>20.79</v>
+        <v>40.095000000000006</v>
       </c>
       <c r="L28" s="1">
         <v>675</v>
@@ -2300,7 +2296,7 @@
         <v>410</v>
       </c>
       <c r="N28" s="1">
-        <f>LOG10(1/M28*1000)*2</f>
+        <f t="shared" si="16"/>
         <v>0.77443228656052898</v>
       </c>
       <c r="O28">
@@ -2312,158 +2308,158 @@
         <v>13.319974733295901</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="Q28:Q29" si="20">P28*N28+P28</f>
         <v>23.635393222930716</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C29" s="3">
-        <v>2150</v>
+        <v>2350</v>
       </c>
       <c r="D29" s="4">
-        <f>C29/14</f>
-        <v>153.57142857142858</v>
+        <f t="shared" si="14"/>
+        <v>156.66666666666666</v>
       </c>
       <c r="E29" s="9">
-        <f t="shared" si="20"/>
-        <v>0.15793953488372092</v>
+        <f t="shared" ref="E29:E36" si="21">K29/D29</f>
+        <v>0.13270212765957448</v>
       </c>
       <c r="F29" s="8">
         <f t="shared" si="2"/>
-        <v>0.23441860465116277</v>
+        <v>0.24255319148936172</v>
       </c>
       <c r="G29" s="3">
-        <v>0.36</v>
+        <v>0.38</v>
       </c>
       <c r="H29" s="3">
-        <v>1.05</v>
+        <v>0.7</v>
       </c>
       <c r="I29">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="J29">
-        <f t="shared" si="18"/>
-        <v>0.36749999999999999</v>
+        <f t="shared" si="19"/>
+        <v>0.315</v>
       </c>
       <c r="K29" s="2">
         <f>J29*Feuil2!$B$1</f>
-        <v>24.254999999999999</v>
+        <v>20.79</v>
       </c>
       <c r="L29" s="1">
-        <v>570</v>
+        <v>675</v>
       </c>
       <c r="M29" s="1">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="N29" s="1">
-        <f>LOG10(1/M29*1000)*2</f>
-        <v>0.81787078594700169</v>
+        <f t="shared" si="16"/>
+        <v>0.77443228656052898</v>
       </c>
       <c r="O29">
         <f>L29/Feuil2!$B$2</f>
-        <v>0.16002245929253228</v>
+        <v>0.18950028074115666</v>
       </c>
       <c r="P29">
         <f>O29*Feuil2!$B$3</f>
-        <v>11.247978663672093</v>
+        <v>13.319974733295901</v>
       </c>
       <c r="Q29">
-        <f t="shared" ref="Q29" si="21">P29*N29+P29</f>
-        <v>20.447371813644693</v>
+        <f t="shared" si="20"/>
+        <v>23.635393222930716</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C30" s="3">
+        <v>2150</v>
+      </c>
+      <c r="D30" s="4">
+        <f>C30/14</f>
+        <v>153.57142857142858</v>
+      </c>
+      <c r="E30" s="9">
+        <f t="shared" si="21"/>
+        <v>0.15793953488372092</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" si="2"/>
+        <v>0.2409302325581395</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1.05</v>
+      </c>
+      <c r="I30">
+        <v>0.35</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="19"/>
+        <v>0.36749999999999999</v>
+      </c>
+      <c r="K30" s="2">
+        <f>J30*Feuil2!$B$1</f>
+        <v>24.254999999999999</v>
+      </c>
+      <c r="L30" s="1">
+        <v>570</v>
+      </c>
+      <c r="M30" s="1">
+        <v>390</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="16"/>
+        <v>0.81787078594700169</v>
+      </c>
+      <c r="O30">
+        <f>L30/Feuil2!$B$2</f>
+        <v>0.16002245929253228</v>
+      </c>
+      <c r="P30">
+        <f>O30*Feuil2!$B$3</f>
+        <v>11.247978663672093</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" ref="Q30" si="22">P30*N30+P30</f>
+        <v>20.447371813644693</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="3">
         <v>2600</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D31" s="4">
         <f t="shared" si="14"/>
         <v>173.33333333333334</v>
       </c>
-      <c r="E30" s="9">
-        <f t="shared" si="20"/>
+      <c r="E31" s="9">
+        <f t="shared" si="21"/>
         <v>0.13136538461538461</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F31" s="8">
         <f t="shared" si="2"/>
         <v>0.24230769230769228</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G31" s="3">
         <v>0.42</v>
-      </c>
-      <c r="H30" s="3">
-        <v>0.69</v>
-      </c>
-      <c r="I30">
-        <v>0.5</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="18"/>
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="K30" s="2">
-        <f>J30*Feuil2!$B$1</f>
-        <v>22.77</v>
-      </c>
-      <c r="L30" s="1">
-        <v>538</v>
-      </c>
-      <c r="M30" s="1">
-        <v>850</v>
-      </c>
-      <c r="N30" s="1">
-        <f>LOG10(1/M30*1000)*2</f>
-        <v>0.1411621485714144</v>
-      </c>
-      <c r="O30">
-        <f>L30/Feuil2!$B$2</f>
-        <v>0.15103874227961819</v>
-      </c>
-      <c r="P30">
-        <f>O30*Feuil2!$B$3</f>
-        <v>10.616513194834361</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" ref="Q30" si="22">P30*N30+P30</f>
-        <v>12.115163007753951</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="3">
-        <v>1275</v>
-      </c>
-      <c r="D31" s="4">
-        <f t="shared" si="14"/>
-        <v>85</v>
-      </c>
-      <c r="E31" s="9">
-        <f t="shared" si="20"/>
-        <v>0.26788235294117646</v>
-      </c>
-      <c r="F31" s="9">
-        <f t="shared" si="2"/>
-        <v>0.24705882352941178</v>
-      </c>
-      <c r="G31" s="3">
-        <v>0.21</v>
       </c>
       <c r="H31" s="3">
         <v>0.69</v>
@@ -2472,7 +2468,7 @@
         <v>0.5</v>
       </c>
       <c r="J31">
-        <f t="shared" ref="J31" si="23">I31*H31</f>
+        <f t="shared" si="19"/>
         <v>0.34499999999999997</v>
       </c>
       <c r="K31" s="2">
@@ -2486,7 +2482,7 @@
         <v>850</v>
       </c>
       <c r="N31" s="1">
-        <f>LOG10(1/M31*1000)*2</f>
+        <f t="shared" si="16"/>
         <v>0.1411621485714144</v>
       </c>
       <c r="O31">
@@ -2498,111 +2494,111 @@
         <v>10.616513194834361</v>
       </c>
       <c r="Q31">
-        <f t="shared" ref="Q31" si="24">P31*N31+P31</f>
+        <f t="shared" ref="Q31" si="23">P31*N31+P31</f>
         <v>12.115163007753951</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1275</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="14"/>
+        <v>85</v>
+      </c>
+      <c r="E32" s="9">
+        <f t="shared" si="21"/>
+        <v>0.26788235294117646</v>
+      </c>
+      <c r="F32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.24705882352941178</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="I32">
+        <v>0.5</v>
+      </c>
+      <c r="J32">
+        <f t="shared" ref="J32" si="24">I32*H32</f>
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="K32" s="2">
+        <f>J32*Feuil2!$B$1</f>
+        <v>22.77</v>
+      </c>
+      <c r="L32" s="1">
+        <v>538</v>
+      </c>
+      <c r="M32" s="1">
+        <v>850</v>
+      </c>
+      <c r="N32" s="1">
+        <f t="shared" si="16"/>
+        <v>0.1411621485714144</v>
+      </c>
+      <c r="O32">
+        <f>L32/Feuil2!$B$2</f>
+        <v>0.15103874227961819</v>
+      </c>
+      <c r="P32">
+        <f>O32*Feuil2!$B$3</f>
+        <v>10.616513194834361</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" ref="Q32" si="25">P32*N32+P32</f>
+        <v>12.115163007753951</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C33" s="3">
         <v>875</v>
       </c>
-      <c r="D32" s="4">
-        <f>C32/16</f>
+      <c r="D33" s="4">
+        <f>C33/16</f>
         <v>54.6875</v>
       </c>
-      <c r="E32" s="10">
-        <f t="shared" si="20"/>
+      <c r="E33" s="10">
+        <f t="shared" si="21"/>
         <v>0.54362879999999991</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F33" s="9">
         <f t="shared" si="2"/>
         <v>0.1462857142857143</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G33" s="3">
         <v>0.08</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H33" s="3">
         <f>0.7*1.43</f>
         <v>1.0009999999999999</v>
       </c>
-      <c r="I32">
-        <v>0.45</v>
-      </c>
-      <c r="J32">
-        <f t="shared" ref="J32" si="25">I32*H32</f>
-        <v>0.45044999999999996</v>
-      </c>
-      <c r="K32" s="2">
-        <f>J32*Feuil2!$B$1</f>
-        <v>29.729699999999998</v>
-      </c>
-      <c r="L32" s="1">
-        <v>697</v>
-      </c>
-      <c r="M32" s="1">
-        <v>497</v>
-      </c>
-      <c r="N32" s="1">
-        <f t="shared" ref="N32:N35" si="26">LOG10(1/M32*1000)*2</f>
-        <v>0.60728722253333589</v>
-      </c>
-      <c r="O32">
-        <f>L32/Feuil2!$B$2</f>
-        <v>0.19567658618753508</v>
-      </c>
-      <c r="P32">
-        <f>O32*Feuil2!$B$3</f>
-        <v>13.75410724312184</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" ref="Q32:Q33" si="27">P32*N32+P32</f>
-        <v>22.106800829222941</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="3">
-        <v>975</v>
-      </c>
-      <c r="D33" s="4">
-        <f>C33/16</f>
-        <v>60.9375</v>
-      </c>
-      <c r="E33" s="9">
-        <f t="shared" si="20"/>
-        <v>0.34116923076923078</v>
-      </c>
-      <c r="F33" s="8">
-        <f t="shared" si="2"/>
-        <v>0.41025641025641024</v>
-      </c>
-      <c r="G33">
-        <v>0.25</v>
-      </c>
-      <c r="H33" s="3">
-        <v>0.7</v>
-      </c>
       <c r="I33">
         <v>0.45</v>
       </c>
       <c r="J33">
-        <f t="shared" ref="J33:J34" si="28">I33*H33</f>
-        <v>0.315</v>
+        <f t="shared" ref="J33" si="26">I33*H33</f>
+        <v>0.45044999999999996</v>
       </c>
       <c r="K33" s="2">
         <f>J33*Feuil2!$B$1</f>
-        <v>20.79</v>
+        <v>29.729699999999998</v>
       </c>
       <c r="L33" s="1">
         <v>697</v>
@@ -2611,7 +2607,7 @@
         <v>497</v>
       </c>
       <c r="N33" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="N33:N36" si="27">LOG10(1/M33*1000)*2</f>
         <v>0.60728722253333589</v>
       </c>
       <c r="O33">
@@ -2623,110 +2619,110 @@
         <v>13.75410724312184</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="Q33:Q34" si="28">P33*N33+P33</f>
         <v>22.106800829222941</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" t="s">
-        <v>56</v>
+      <c r="A34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C34" s="3">
-        <v>950</v>
+        <v>975</v>
       </c>
       <c r="D34" s="4">
-        <f>C34/14</f>
-        <v>67.857142857142861</v>
+        <f>C34/16</f>
+        <v>60.9375</v>
       </c>
       <c r="E34" s="9">
-        <f t="shared" si="20"/>
-        <v>0.37446315789473683</v>
-      </c>
-      <c r="F34" s="9">
-        <f t="shared" si="2"/>
-        <v>0.27999999999999997</v>
+        <f t="shared" si="21"/>
+        <v>0.34116923076923078</v>
+      </c>
+      <c r="F34" s="8">
+        <f t="shared" si="2"/>
+        <v>0.41025641025641024</v>
       </c>
       <c r="G34">
-        <v>0.19</v>
+        <v>0.25</v>
       </c>
       <c r="H34" s="3">
         <v>0.7</v>
       </c>
       <c r="I34">
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
       <c r="J34">
-        <f t="shared" si="28"/>
-        <v>0.38500000000000001</v>
+        <f t="shared" ref="J34:J35" si="29">I34*H34</f>
+        <v>0.315</v>
       </c>
       <c r="K34" s="2">
         <f>J34*Feuil2!$B$1</f>
-        <v>25.41</v>
+        <v>20.79</v>
       </c>
       <c r="L34" s="1">
-        <v>559</v>
+        <v>697</v>
       </c>
       <c r="M34" s="1">
-        <v>320</v>
+        <v>497</v>
       </c>
       <c r="N34" s="1">
-        <f t="shared" si="26"/>
-        <v>0.98970004336018802</v>
+        <f t="shared" si="27"/>
+        <v>0.60728722253333589</v>
       </c>
       <c r="O34">
         <f>L34/Feuil2!$B$2</f>
-        <v>0.15693430656934307</v>
+        <v>0.19567658618753508</v>
       </c>
       <c r="P34">
         <f>O34*Feuil2!$B$3</f>
-        <v>11.030912408759123</v>
+        <v>13.75410724312184</v>
       </c>
       <c r="Q34">
-        <f t="shared" ref="Q34" si="29">P34*N34+P34</f>
-        <v>21.948206898010461</v>
+        <f t="shared" si="28"/>
+        <v>22.106800829222941</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>55</v>
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
       </c>
       <c r="C35" s="3">
-        <v>1750</v>
+        <v>950</v>
       </c>
       <c r="D35" s="4">
         <f>C35/14</f>
-        <v>125</v>
-      </c>
-      <c r="E35" s="10">
-        <f t="shared" si="20"/>
-        <v>0.58080000000000009</v>
+        <v>67.857142857142861</v>
+      </c>
+      <c r="E35" s="9">
+        <f t="shared" si="21"/>
+        <v>0.37446315789473683</v>
       </c>
       <c r="F35" s="9">
         <f t="shared" si="2"/>
-        <v>0.08</v>
+        <v>0.27999999999999997</v>
       </c>
       <c r="G35">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="H35" s="3">
-        <v>2</v>
+        <v>0.7</v>
       </c>
       <c r="I35">
         <v>0.55000000000000004</v>
       </c>
       <c r="J35">
-        <f t="shared" ref="J35:J36" si="30">I35*H35</f>
-        <v>1.1000000000000001</v>
+        <f t="shared" si="29"/>
+        <v>0.38500000000000001</v>
       </c>
       <c r="K35" s="2">
         <f>J35*Feuil2!$B$1</f>
-        <v>72.600000000000009</v>
+        <v>25.41</v>
       </c>
       <c r="L35" s="1">
         <v>559</v>
@@ -2735,7 +2731,7 @@
         <v>320</v>
       </c>
       <c r="N35" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.98970004336018802</v>
       </c>
       <c r="O35">
@@ -2747,88 +2743,316 @@
         <v>11.030912408759123</v>
       </c>
       <c r="Q35">
-        <f t="shared" ref="Q35" si="31">P35*N35+P35</f>
+        <f t="shared" ref="Q35" si="30">P35*N35+P35</f>
         <v>21.948206898010461</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36">
-        <v>5250</v>
+      <c r="A36" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1750</v>
       </c>
       <c r="D36" s="4">
-        <f>C36/10</f>
-        <v>525</v>
+        <f>C36/14</f>
+        <v>125</v>
       </c>
       <c r="E36" s="10">
-        <f>K36/D36</f>
-        <v>0.12068571428571429</v>
+        <f t="shared" si="21"/>
+        <v>0.58080000000000009</v>
       </c>
       <c r="F36" s="9">
         <f t="shared" si="2"/>
-        <v>8.5714285714285715E-2</v>
+        <v>0.08</v>
       </c>
       <c r="G36">
-        <v>0.45</v>
+        <v>0.1</v>
       </c>
       <c r="H36" s="3">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="I36">
-        <v>0.8</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J36">
-        <f t="shared" si="30"/>
-        <v>0.96</v>
+        <f t="shared" ref="J36:J37" si="31">I36*H36</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K36" s="2">
         <f>J36*Feuil2!$B$1</f>
-        <v>63.36</v>
+        <v>72.600000000000009</v>
+      </c>
+      <c r="L36" s="1">
+        <v>559</v>
+      </c>
+      <c r="M36" s="1">
+        <v>320</v>
+      </c>
+      <c r="N36" s="1">
+        <f t="shared" si="27"/>
+        <v>0.98970004336018802</v>
+      </c>
+      <c r="O36">
+        <f>L36/Feuil2!$B$2</f>
+        <v>0.15693430656934307</v>
+      </c>
+      <c r="P36">
+        <f>O36*Feuil2!$B$3</f>
+        <v>11.030912408759123</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" ref="Q36" si="32">P36*N36+P36</f>
+        <v>21.948206898010461</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C37">
-        <v>1250</v>
+        <v>5000</v>
       </c>
       <c r="D37" s="4">
         <f>C37/10</f>
-        <v>125</v>
+        <v>500</v>
       </c>
       <c r="E37" s="10">
-        <f t="shared" ref="E37" si="32">K37/D37</f>
-        <v>0.84480000000000011</v>
+        <f>K37/D37</f>
+        <v>0.14783999999999997</v>
       </c>
       <c r="F37" s="9">
-        <f t="shared" ref="F37" si="33">G37/D37*100</f>
-        <v>0.184</v>
+        <f t="shared" si="2"/>
+        <v>8.3999999999999991E-2</v>
       </c>
       <c r="G37">
-        <v>0.23</v>
+        <v>0.42</v>
       </c>
       <c r="H37" s="3">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="I37">
         <v>0.8</v>
       </c>
       <c r="J37">
-        <f t="shared" ref="J37" si="34">I37*H37</f>
-        <v>1.6</v>
+        <f t="shared" si="31"/>
+        <v>1.1199999999999999</v>
       </c>
       <c r="K37" s="2">
         <f>J37*Feuil2!$B$1</f>
-        <v>105.60000000000001</v>
+        <v>73.919999999999987</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38">
+        <v>1450</v>
+      </c>
+      <c r="D38" s="4">
+        <f>C38/10</f>
+        <v>145</v>
+      </c>
+      <c r="E38" s="10">
+        <f>K38/D38</f>
+        <v>0.91034482758620694</v>
+      </c>
+      <c r="F38" s="9">
+        <f t="shared" ref="F38:F39" si="33">G38/D38*100</f>
+        <v>0.15862068965517243</v>
+      </c>
+      <c r="G38">
+        <v>0.23</v>
+      </c>
+      <c r="H38" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="I38">
+        <v>0.8</v>
+      </c>
+      <c r="J38">
+        <f t="shared" ref="J38:J39" si="34">I38*H38</f>
+        <v>2</v>
+      </c>
+      <c r="K38" s="2">
+        <f>J38*Feuil2!$B$1</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="3">
+        <v>750</v>
+      </c>
+      <c r="D39" s="4">
+        <f>C39/10</f>
+        <v>75</v>
+      </c>
+      <c r="E39" s="10">
+        <f>K39/D39</f>
+        <v>2.5344000000000002</v>
+      </c>
+      <c r="F39" s="7">
+        <f t="shared" si="33"/>
+        <v>0.36000000000000004</v>
+      </c>
+      <c r="G39">
+        <f>9*0.03</f>
+        <v>0.27</v>
+      </c>
+      <c r="H39">
+        <f>9*0.4</f>
+        <v>3.6</v>
+      </c>
+      <c r="I39">
+        <v>0.8</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="34"/>
+        <v>2.8800000000000003</v>
+      </c>
+      <c r="K39" s="2">
+        <f>J39*Feuil2!$B$1</f>
+        <v>190.08</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40">
+        <v>2000</v>
+      </c>
+      <c r="D40" s="4">
+        <f>C40/10</f>
+        <v>200</v>
+      </c>
+      <c r="E40" s="10">
+        <f>K40/D40</f>
+        <v>1.4256</v>
+      </c>
+      <c r="F40" s="9">
+        <f t="shared" ref="F40:F42" si="35">G40/D40*100</f>
+        <v>0.18</v>
+      </c>
+      <c r="G40">
+        <f>6*0.06</f>
+        <v>0.36</v>
+      </c>
+      <c r="H40" s="3">
+        <f>1.5*6</f>
+        <v>9</v>
+      </c>
+      <c r="I40">
+        <v>0.48</v>
+      </c>
+      <c r="J40">
+        <f t="shared" ref="J40:J42" si="36">I40*H40</f>
+        <v>4.32</v>
+      </c>
+      <c r="K40" s="2">
+        <f>J40*Feuil2!$B$1</f>
+        <v>285.12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41">
+        <v>9500</v>
+      </c>
+      <c r="D41" s="4">
+        <f>C41/10</f>
+        <v>950</v>
+      </c>
+      <c r="E41" s="10">
+        <f>K41/D41</f>
+        <v>0.14005894736842106</v>
+      </c>
+      <c r="F41" s="9">
+        <f t="shared" si="35"/>
+        <v>5.3684210526315793E-2</v>
+      </c>
+      <c r="G41">
+        <v>0.51</v>
+      </c>
+      <c r="H41">
+        <v>4.2</v>
+      </c>
+      <c r="I41">
+        <v>0.48</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="36"/>
+        <v>2.016</v>
+      </c>
+      <c r="K41" s="2">
+        <f>J41*Feuil2!$B$1</f>
+        <v>133.05600000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42">
+        <v>600</v>
+      </c>
+      <c r="D42" s="4">
+        <f>C42/10</f>
+        <v>60</v>
+      </c>
+      <c r="E42" s="10">
+        <f>K42/D42</f>
+        <v>2.3759999999999994</v>
+      </c>
+      <c r="F42" s="9">
+        <f t="shared" si="35"/>
+        <v>0.45000000000000007</v>
+      </c>
+      <c r="G42">
+        <f>9*0.03</f>
+        <v>0.27</v>
+      </c>
+      <c r="H42">
+        <f>9*0.3</f>
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="I42">
+        <v>0.8</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="36"/>
+        <v>2.1599999999999997</v>
+      </c>
+      <c r="K42" s="2">
+        <f>J42*Feuil2!$B$1</f>
+        <v>142.55999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slightly increased Ash12 power
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -579,7 +579,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="E11" s="9">
         <f t="shared" si="1"/>
-        <v>0.26730000000000004</v>
+        <v>0.27324000000000004</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="2"/>
@@ -1224,15 +1224,15 @@
         <v>1.35</v>
       </c>
       <c r="I11">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="J11">
         <f t="shared" si="5"/>
-        <v>1.2150000000000001</v>
+        <v>1.2420000000000002</v>
       </c>
       <c r="K11" s="2">
         <f>J11*Feuil2!$B$1</f>
-        <v>80.190000000000012</v>
+        <v>81.972000000000008</v>
       </c>
       <c r="L11" s="1">
         <v>3307</v>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>0.11621739130434784</v>
+        <v>0.11880000000000002</v>
       </c>
       <c r="F12" s="8">
         <f t="shared" si="2"/>
@@ -1286,15 +1286,15 @@
         <v>1.35</v>
       </c>
       <c r="I12">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="J12">
         <f t="shared" si="5"/>
-        <v>1.2150000000000001</v>
+        <v>1.2420000000000002</v>
       </c>
       <c r="K12" s="2">
         <f>J12*Feuil2!$B$1</f>
-        <v>80.190000000000012</v>
+        <v>81.972000000000008</v>
       </c>
       <c r="L12" s="1">
         <v>3307</v>

</xml_diff>

<commit_message>
7.62x54r FMJ and 7.92 FMJ price and perf matching
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -579,7 +579,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,19 +769,19 @@
         <v>56</v>
       </c>
       <c r="C4">
-        <v>2035</v>
+        <v>2250</v>
       </c>
       <c r="D4" s="4">
         <f>C4/15</f>
-        <v>135.66666666666666</v>
+        <v>150</v>
       </c>
       <c r="E4" s="9">
         <f t="shared" ref="E4:E27" si="1">K4/D4</f>
-        <v>0.57721621621621622</v>
+        <v>0.52205999999999997</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" ref="F4:F37" si="2">G4/D4*100</f>
-        <v>0.18427518427518427</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="G4">
         <v>0.25</v>
@@ -893,22 +893,22 @@
         <v>56</v>
       </c>
       <c r="C6">
-        <v>2700</v>
+        <v>2250</v>
       </c>
       <c r="D6" s="4">
         <f>C6/10</f>
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" si="1"/>
-        <v>0.27345999999999998</v>
+        <v>0.328152</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="2"/>
-        <v>0.10740740740740741</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="G6" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="H6" s="3">
         <v>1.0169999999999999</v>
@@ -955,19 +955,19 @@
         <v>54</v>
       </c>
       <c r="C7">
-        <v>10150</v>
+        <v>9500</v>
       </c>
       <c r="D7" s="4">
         <f>C7/10</f>
-        <v>1015</v>
+        <v>950</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="1"/>
-        <v>7.274305418719211E-2</v>
+        <v>7.7720210526315781E-2</v>
       </c>
       <c r="F7" s="8">
         <f t="shared" si="2"/>
-        <v>7.8817733990147784E-2</v>
+        <v>8.4210526315789472E-2</v>
       </c>
       <c r="G7" s="3">
         <v>0.8</v>

</xml_diff>

<commit_message>
23x75 and other BAS rounds values fix
23x75 got a huge buff, no wonder this was underwhelming in game.
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2981,22 +2981,22 @@
         <v>54</v>
       </c>
       <c r="C41">
-        <v>9500</v>
+        <v>7000</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" si="33"/>
-        <v>950</v>
+        <v>700</v>
       </c>
       <c r="E41" s="10">
         <f t="shared" si="34"/>
-        <v>0.14005894736842106</v>
+        <v>0.19008000000000003</v>
       </c>
       <c r="F41" s="9">
         <f t="shared" si="37"/>
-        <v>5.3684210526315793E-2</v>
+        <v>7.7142857142857152E-2</v>
       </c>
       <c r="G41">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="H41">
         <v>4.2</v>

</xml_diff>

<commit_message>
Slower .45 ammo and a bit less .45 Hydra damage
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.richard\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groki\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2763,7 +2763,7 @@
       </c>
       <c r="E36" s="10">
         <f t="shared" si="21"/>
-        <v>0.65339999999999998</v>
+        <v>0.62145600000000012</v>
       </c>
       <c r="F36" s="9">
         <f t="shared" si="2"/>
@@ -2773,18 +2773,18 @@
         <v>0.1</v>
       </c>
       <c r="H36" s="3">
-        <v>2.25</v>
+        <v>2.14</v>
       </c>
       <c r="I36">
         <v>0.55000000000000004</v>
       </c>
       <c r="J36">
         <f t="shared" ref="J36:J37" si="31">I36*H36</f>
-        <v>1.2375</v>
+        <v>1.1770000000000003</v>
       </c>
       <c r="K36" s="2">
         <f>J36*Feuil2!$B$1</f>
-        <v>81.674999999999997</v>
+        <v>77.682000000000016</v>
       </c>
       <c r="L36" s="1">
         <v>559</v>

</xml_diff>

<commit_message>
9x39 AP and DMG boost
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -579,7 +579,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,28 +1831,28 @@
       </c>
       <c r="E21" s="9">
         <f t="shared" si="1"/>
-        <v>0.36444374999999996</v>
+        <v>0.39896999999999999</v>
       </c>
       <c r="F21" s="9">
         <f t="shared" si="2"/>
-        <v>0.28125</v>
+        <v>0.31875000000000003</v>
       </c>
       <c r="G21" s="3">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
       <c r="H21" s="3">
-        <v>0.95</v>
+        <v>1.04</v>
       </c>
       <c r="I21">
         <v>0.62</v>
       </c>
       <c r="J21">
         <f t="shared" si="9"/>
-        <v>0.58899999999999997</v>
+        <v>0.64480000000000004</v>
       </c>
       <c r="K21" s="2">
         <f>J21*Feuil2!$B$1</f>
-        <v>38.873999999999995</v>
+        <v>42.556800000000003</v>
       </c>
       <c r="L21" s="1">
         <v>964</v>
@@ -1893,28 +1893,28 @@
       </c>
       <c r="E22" s="9">
         <f t="shared" si="1"/>
-        <v>0.11213653846153844</v>
+        <v>0.12275999999999999</v>
       </c>
       <c r="F22" s="8">
         <f t="shared" si="2"/>
-        <v>0.1528846153846154</v>
+        <v>0.15865384615384615</v>
       </c>
       <c r="G22" s="3">
-        <v>0.53</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H22" s="3">
-        <v>0.95</v>
+        <v>1.04</v>
       </c>
       <c r="I22">
         <v>0.62</v>
       </c>
       <c r="J22">
         <f t="shared" ref="J22" si="10">I22*H22</f>
-        <v>0.58899999999999997</v>
+        <v>0.64480000000000004</v>
       </c>
       <c r="K22" s="2">
         <f>J22*Feuil2!$B$1</f>
-        <v>38.873999999999995</v>
+        <v>42.556800000000003</v>
       </c>
       <c r="L22" s="1">
         <v>964</v>

</xml_diff>

<commit_message>
Reduced hydro damage to 69
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -579,7 +579,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2763,7 +2763,7 @@
       </c>
       <c r="E36" s="10">
         <f t="shared" si="21"/>
-        <v>0.62145600000000012</v>
+        <v>0.54885600000000001</v>
       </c>
       <c r="F36" s="9">
         <f t="shared" si="2"/>
@@ -2773,18 +2773,18 @@
         <v>0.1</v>
       </c>
       <c r="H36" s="3">
-        <v>2.14</v>
+        <v>1.89</v>
       </c>
       <c r="I36">
         <v>0.55000000000000004</v>
       </c>
       <c r="J36">
         <f t="shared" ref="J36:J37" si="31">I36*H36</f>
-        <v>1.1770000000000003</v>
+        <v>1.0395000000000001</v>
       </c>
       <c r="K36" s="2">
         <f>J36*Feuil2!$B$1</f>
-        <v>77.682000000000016</v>
+        <v>68.606999999999999</v>
       </c>
       <c r="L36" s="1">
         <v>559</v>

</xml_diff>

<commit_message>
Sniper rounds damage nerf
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groki\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.richard\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -579,7 +579,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +672,7 @@
       </c>
       <c r="E2" s="9">
         <f>K2/D2</f>
-        <v>7.640470588235293E-2</v>
+        <v>5.8701176470588236E-2</v>
       </c>
       <c r="F2" s="8">
         <f>G2/D2*100</f>
@@ -682,18 +682,18 @@
         <v>1.4</v>
       </c>
       <c r="H2" s="3">
-        <v>1.64</v>
+        <v>1.26</v>
       </c>
       <c r="I2">
         <v>1.2</v>
       </c>
       <c r="J2">
         <f>H2*I2</f>
-        <v>1.9679999999999997</v>
+        <v>1.512</v>
       </c>
       <c r="K2" s="2">
         <f>J2*Feuil2!$B$1</f>
-        <v>129.88799999999998</v>
+        <v>99.792000000000002</v>
       </c>
       <c r="L2" s="1">
         <v>6931</v>
@@ -777,7 +777,7 @@
       </c>
       <c r="E4" s="9">
         <f t="shared" ref="E4:E27" si="1">K4/D4</f>
-        <v>0.52205999999999997</v>
+        <v>0.46199999999999997</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" ref="F4:F37" si="2">G4/D4*100</f>
@@ -787,18 +787,18 @@
         <v>0.25</v>
       </c>
       <c r="H4" s="3">
-        <v>1.1299999999999999</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>1.05</v>
       </c>
       <c r="J4">
         <f>I4*H4</f>
-        <v>1.1864999999999999</v>
+        <v>1.05</v>
       </c>
       <c r="K4" s="2">
         <f>J4*Feuil2!$B$1</f>
-        <v>78.308999999999997</v>
+        <v>69.3</v>
       </c>
       <c r="L4" s="1">
         <v>4064</v>
@@ -839,7 +839,7 @@
       </c>
       <c r="E5" s="9">
         <f t="shared" si="1"/>
-        <v>0.16780499999999998</v>
+        <v>0.14849999999999999</v>
       </c>
       <c r="F5" s="8">
         <f t="shared" si="2"/>
@@ -849,18 +849,18 @@
         <v>0.39</v>
       </c>
       <c r="H5" s="3">
-        <v>1.1299999999999999</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>1.05</v>
       </c>
       <c r="J5">
         <f>I5*H5</f>
-        <v>1.1864999999999999</v>
+        <v>1.05</v>
       </c>
       <c r="K5" s="2">
         <f>J5*Feuil2!$B$1</f>
-        <v>78.308999999999997</v>
+        <v>69.3</v>
       </c>
       <c r="L5" s="1">
         <v>4064</v>
@@ -901,7 +901,7 @@
       </c>
       <c r="E6" s="9">
         <f t="shared" si="1"/>
-        <v>0.328152</v>
+        <v>0.27426666666666666</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="2"/>
@@ -911,18 +911,18 @@
         <v>0.3</v>
       </c>
       <c r="H6" s="3">
-        <v>1.0169999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="I6">
         <v>1.1000000000000001</v>
       </c>
       <c r="J6">
         <f t="shared" ref="J6:J19" si="5">I6*H6</f>
-        <v>1.1187</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="K6" s="2">
         <f>J6*Feuil2!$B$1</f>
-        <v>73.834199999999996</v>
+        <v>61.71</v>
       </c>
       <c r="L6" s="1">
         <v>3744</v>
@@ -963,7 +963,7 @@
       </c>
       <c r="E7" s="9">
         <f t="shared" si="1"/>
-        <v>7.7720210526315781E-2</v>
+        <v>6.4957894736842103E-2</v>
       </c>
       <c r="F7" s="8">
         <f t="shared" si="2"/>
@@ -973,18 +973,18 @@
         <v>0.8</v>
       </c>
       <c r="H7" s="3">
-        <v>1.0169999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="I7">
         <v>1.1000000000000001</v>
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
-        <v>1.1187</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="K7" s="2">
         <f>J7*Feuil2!$B$1</f>
-        <v>73.834199999999996</v>
+        <v>61.71</v>
       </c>
       <c r="L7" s="1">
         <v>3744</v>
@@ -1025,7 +1025,7 @@
       </c>
       <c r="E8" s="9">
         <f t="shared" si="1"/>
-        <v>0.18458549999999999</v>
+        <v>0.154275</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="2"/>
@@ -1035,18 +1035,18 @@
         <v>0.45</v>
       </c>
       <c r="H8" s="3">
-        <v>1.0169999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="I8">
         <v>1.1000000000000001</v>
       </c>
       <c r="J8">
         <f t="shared" si="5"/>
-        <v>1.1187</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="K8" s="2">
         <f>J8*Feuil2!$B$1</f>
-        <v>73.834199999999996</v>
+        <v>61.71</v>
       </c>
       <c r="L8" s="1">
         <v>3744</v>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="E9" s="9">
         <f t="shared" si="1"/>
-        <v>0.35144999999999998</v>
+        <v>0.29370000000000002</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="2"/>
@@ -1097,18 +1097,18 @@
         <v>0.34</v>
       </c>
       <c r="H9" s="3">
-        <v>1.0649999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" si="5"/>
-        <v>1.0649999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="K9" s="2">
         <f>J9*Feuil2!$B$1</f>
-        <v>70.289999999999992</v>
+        <v>58.74</v>
       </c>
       <c r="L9" s="1">
         <v>3562</v>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="E10" s="9">
         <f t="shared" si="1"/>
-        <v>0.14057999999999998</v>
+        <v>0.11748</v>
       </c>
       <c r="F10" s="8">
         <f t="shared" si="2"/>
@@ -1159,18 +1159,18 @@
         <v>0.62</v>
       </c>
       <c r="H10" s="3">
-        <v>1.0649999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
         <f t="shared" si="5"/>
-        <v>1.0649999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="K10" s="2">
         <f>J10*Feuil2!$B$1</f>
-        <v>70.289999999999992</v>
+        <v>58.74</v>
       </c>
       <c r="L10" s="1">
         <v>3562</v>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="E11" s="9">
         <f t="shared" si="1"/>
-        <v>0.27324000000000004</v>
+        <v>0.24288000000000001</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="2"/>
@@ -1221,18 +1221,18 @@
         <v>0.38</v>
       </c>
       <c r="H11" s="3">
-        <v>1.35</v>
+        <v>1.2</v>
       </c>
       <c r="I11">
         <v>0.92</v>
       </c>
       <c r="J11">
         <f t="shared" si="5"/>
-        <v>1.2420000000000002</v>
+        <v>1.1040000000000001</v>
       </c>
       <c r="K11" s="2">
         <f>J11*Feuil2!$B$1</f>
-        <v>81.972000000000008</v>
+        <v>72.864000000000004</v>
       </c>
       <c r="L11" s="1">
         <v>3307</v>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>0.11880000000000002</v>
+        <v>0.1056</v>
       </c>
       <c r="F12" s="8">
         <f t="shared" si="2"/>
@@ -1283,18 +1283,18 @@
         <v>0.75</v>
       </c>
       <c r="H12" s="3">
-        <v>1.35</v>
+        <v>1.2</v>
       </c>
       <c r="I12">
         <v>0.92</v>
       </c>
       <c r="J12">
         <f t="shared" si="5"/>
-        <v>1.2420000000000002</v>
+        <v>1.1040000000000001</v>
       </c>
       <c r="K12" s="2">
         <f>J12*Feuil2!$B$1</f>
-        <v>81.972000000000008</v>
+        <v>72.864000000000004</v>
       </c>
       <c r="L12" s="1">
         <v>3307</v>

</xml_diff>

<commit_message>
.45 ACP AP boosted to 21 and DMG to 27
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.richard\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groki\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -579,7 +579,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2701,28 +2701,28 @@
       </c>
       <c r="E35" s="9">
         <f t="shared" si="21"/>
-        <v>0.37446315789473683</v>
+        <v>0.39586105263157895</v>
       </c>
       <c r="F35" s="9">
         <f t="shared" si="2"/>
-        <v>0.27999999999999997</v>
+        <v>0.30947368421052629</v>
       </c>
       <c r="G35">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="H35" s="3">
-        <v>0.7</v>
+        <v>0.74</v>
       </c>
       <c r="I35">
         <v>0.55000000000000004</v>
       </c>
       <c r="J35">
         <f t="shared" si="29"/>
-        <v>0.38500000000000001</v>
+        <v>0.40700000000000003</v>
       </c>
       <c r="K35" s="2">
         <f>J35*Feuil2!$B$1</f>
-        <v>25.41</v>
+        <v>26.862000000000002</v>
       </c>
       <c r="L35" s="1">
         <v>559</v>

</xml_diff>

<commit_message>
5.45 FMJ Buff (27 AP, 38 DMG)
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -579,7 +579,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,28 +1335,28 @@
       </c>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>0.40333333333333338</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="2"/>
-        <v>0.27777777777777779</v>
+        <v>0.3</v>
       </c>
       <c r="G13" s="3">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="H13" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I13">
         <v>0.5</v>
       </c>
       <c r="J13">
         <f t="shared" si="5"/>
-        <v>0.55000000000000004</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="K13" s="2">
         <f>J13*Feuil2!$B$1</f>
-        <v>36.300000000000004</v>
+        <v>37.619999999999997</v>
       </c>
       <c r="L13" s="1">
         <v>1461</v>

</xml_diff>

<commit_message>
Increased Slugs and Buckshot damages
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -579,7 +579,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="E38" s="10">
         <f t="shared" si="34"/>
-        <v>0.91034482758620694</v>
+        <v>0.98317241379310349</v>
       </c>
       <c r="F38" s="9">
         <f t="shared" ref="F38:F39" si="35">G38/D38*100</f>
@@ -2875,18 +2875,18 @@
         <v>0.23</v>
       </c>
       <c r="H38" s="3">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="I38">
         <v>0.8</v>
       </c>
       <c r="J38">
         <f t="shared" ref="J38:J39" si="36">I38*H38</f>
-        <v>2</v>
+        <v>2.16</v>
       </c>
       <c r="K38" s="2">
         <f>J38*Feuil2!$B$1</f>
-        <v>132</v>
+        <v>142.56</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2905,7 +2905,7 @@
       </c>
       <c r="E39" s="10">
         <f t="shared" si="34"/>
-        <v>2.5344000000000002</v>
+        <v>2.6611199999999999</v>
       </c>
       <c r="F39" s="7">
         <f t="shared" si="35"/>
@@ -2916,19 +2916,19 @@
         <v>0.27</v>
       </c>
       <c r="H39">
-        <f>9*0.4</f>
-        <v>3.6</v>
+        <f>9*0.42</f>
+        <v>3.78</v>
       </c>
       <c r="I39">
         <v>0.8</v>
       </c>
       <c r="J39">
         <f t="shared" si="36"/>
-        <v>2.8800000000000003</v>
+        <v>3.024</v>
       </c>
       <c r="K39" s="2">
         <f>J39*Feuil2!$B$1</f>
-        <v>190.08</v>
+        <v>199.584</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "Increased Slugs and Buckshot damages"
This reverts commit b1fb0392b9a60f28c2cf5bc53e2ec5be77a6fd28.
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -579,7 +579,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="E38" s="10">
         <f t="shared" si="34"/>
-        <v>0.98317241379310349</v>
+        <v>0.91034482758620694</v>
       </c>
       <c r="F38" s="9">
         <f t="shared" ref="F38:F39" si="35">G38/D38*100</f>
@@ -2875,18 +2875,18 @@
         <v>0.23</v>
       </c>
       <c r="H38" s="3">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="I38">
         <v>0.8</v>
       </c>
       <c r="J38">
         <f t="shared" ref="J38:J39" si="36">I38*H38</f>
-        <v>2.16</v>
+        <v>2</v>
       </c>
       <c r="K38" s="2">
         <f>J38*Feuil2!$B$1</f>
-        <v>142.56</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2905,7 +2905,7 @@
       </c>
       <c r="E39" s="10">
         <f t="shared" si="34"/>
-        <v>2.6611199999999999</v>
+        <v>2.5344000000000002</v>
       </c>
       <c r="F39" s="7">
         <f t="shared" si="35"/>
@@ -2916,19 +2916,19 @@
         <v>0.27</v>
       </c>
       <c r="H39">
-        <f>9*0.42</f>
-        <v>3.78</v>
+        <f>9*0.4</f>
+        <v>3.6</v>
       </c>
       <c r="I39">
         <v>0.8</v>
       </c>
       <c r="J39">
         <f t="shared" si="36"/>
-        <v>3.024</v>
+        <v>2.8800000000000003</v>
       </c>
       <c r="K39" s="2">
         <f>J39*Feuil2!$B$1</f>
-        <v>199.584</v>
+        <v>190.08</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
.338 federal as mutant hunter + 7.62x54r PP increased damage + text
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\groki\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.richard\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t>ammo_magnum_300</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>ammo_12x70_buck</t>
+  </si>
+  <si>
+    <t>ammo_pkm_100</t>
   </si>
 </sst>
 </file>
@@ -227,7 +230,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +264,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4EC9B0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -282,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -296,6 +311,12 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,28 +755,28 @@
       </c>
       <c r="E3" s="9">
         <f>K3/D3</f>
-        <v>8.5000000000000006E-2</v>
+        <v>0.32129999999999992</v>
       </c>
       <c r="F3" s="8">
         <f>G3/D3*100</f>
-        <v>0.11363636363636363</v>
+        <v>2.7272727272727275E-2</v>
       </c>
       <c r="G3">
-        <v>0.75</v>
+        <v>0.18</v>
       </c>
       <c r="H3" s="3">
-        <v>1</v>
+        <v>3.78</v>
       </c>
       <c r="I3">
         <v>0.85</v>
       </c>
       <c r="J3">
         <f>H3*I3</f>
-        <v>0.85</v>
+        <v>3.2129999999999996</v>
       </c>
       <c r="K3" s="2">
         <f>J3*Feuil2!$B$1</f>
-        <v>56.1</v>
+        <v>212.05799999999996</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2763,7 +2784,7 @@
       </c>
       <c r="E36" s="10">
         <f t="shared" si="21"/>
-        <v>0.54885600000000001</v>
+        <v>0.50239199999999995</v>
       </c>
       <c r="F36" s="9">
         <f t="shared" si="2"/>
@@ -2773,18 +2794,18 @@
         <v>0.1</v>
       </c>
       <c r="H36" s="3">
-        <v>1.89</v>
+        <v>1.73</v>
       </c>
       <c r="I36">
         <v>0.55000000000000004</v>
       </c>
       <c r="J36">
         <f t="shared" ref="J36:J37" si="31">I36*H36</f>
-        <v>1.0395000000000001</v>
+        <v>0.95150000000000001</v>
       </c>
       <c r="K36" s="2">
         <f>J36*Feuil2!$B$1</f>
-        <v>68.606999999999999</v>
+        <v>62.798999999999999</v>
       </c>
       <c r="L36" s="1">
         <v>559</v>
@@ -2824,7 +2845,7 @@
         <v>500</v>
       </c>
       <c r="E37" s="10">
-        <f t="shared" ref="E37:E42" si="34">K37/D37</f>
+        <f t="shared" ref="E37:E43" si="34">K37/D37</f>
         <v>0.14783999999999997</v>
       </c>
       <c r="F37" s="9">
@@ -2950,7 +2971,7 @@
         <v>1.4256</v>
       </c>
       <c r="F40" s="9">
-        <f t="shared" ref="F40:F42" si="37">G40/D40*100</f>
+        <f t="shared" ref="F40:F43" si="37">G40/D40*100</f>
         <v>0.18</v>
       </c>
       <c r="G40">
@@ -2965,7 +2986,7 @@
         <v>0.48</v>
       </c>
       <c r="J40">
-        <f t="shared" ref="J40:J42" si="38">I40*H40</f>
+        <f t="shared" ref="J40:J43" si="38">I40*H40</f>
         <v>4.32</v>
       </c>
       <c r="K40" s="2">
@@ -3055,9 +3076,49 @@
         <v>142.55999999999997</v>
       </c>
     </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="12">
+        <v>5000</v>
+      </c>
+      <c r="D43" s="4">
+        <f>C43/30</f>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="E43" s="10">
+        <f t="shared" si="34"/>
+        <v>0.31101840000000003</v>
+      </c>
+      <c r="F43" s="9">
+        <f t="shared" si="37"/>
+        <v>0.22200000000000003</v>
+      </c>
+      <c r="G43">
+        <v>0.37</v>
+      </c>
+      <c r="H43">
+        <v>1.02</v>
+      </c>
+      <c r="I43">
+        <v>0.77</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="38"/>
+        <v>0.78539999999999999</v>
+      </c>
+      <c r="K43" s="2">
+        <f>J43*Feuil2!$B$1</f>
+        <v>51.836399999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Tripled rockets damage to NPCs, increased price to 12k
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.richard\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t>ammo_magnum_300</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>ammo_pkm_100</t>
+  </si>
+  <si>
+    <t>ammo_og-7b</t>
+  </si>
+  <si>
+    <t>EX</t>
   </si>
 </sst>
 </file>
@@ -597,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2102,7 @@
         <v>960</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" ref="D25:D32" si="14">C25/15</f>
+        <f t="shared" ref="D25:D29" si="14">C25/15</f>
         <v>64</v>
       </c>
       <c r="E25" s="10">
@@ -3114,6 +3120,46 @@
       <c r="K43" s="2">
         <f>J43*Feuil2!$B$1</f>
         <v>51.836399999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44">
+        <v>12490</v>
+      </c>
+      <c r="D44" s="4">
+        <f>C44/30</f>
+        <v>416.33333333333331</v>
+      </c>
+      <c r="E44" s="10">
+        <f t="shared" ref="E44" si="39">K44/D44</f>
+        <v>1.4267413931144917</v>
+      </c>
+      <c r="F44" s="9">
+        <f t="shared" ref="F44" si="40">G44/D44*100</f>
+        <v>8.8871096877502012E-2</v>
+      </c>
+      <c r="G44">
+        <v>0.37</v>
+      </c>
+      <c r="H44">
+        <v>3</v>
+      </c>
+      <c r="I44">
+        <v>3</v>
+      </c>
+      <c r="J44">
+        <f t="shared" ref="J44" si="41">I44*H44</f>
+        <v>9</v>
+      </c>
+      <c r="K44" s="2">
+        <f>J44*Feuil2!$B$1</f>
+        <v>594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
7.62x39 damage increased from 40 to 45
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.richard\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="E19" s="9">
         <f t="shared" si="1"/>
-        <v>0.30918461538461539</v>
+        <v>0.34451999999999994</v>
       </c>
       <c r="F19" s="9">
         <f t="shared" si="2"/>
@@ -1744,18 +1744,18 @@
         <v>0.3</v>
       </c>
       <c r="H19" s="3">
-        <v>1.05</v>
+        <v>1.17</v>
       </c>
       <c r="I19">
         <v>0.57999999999999996</v>
       </c>
       <c r="J19">
         <f t="shared" si="5"/>
-        <v>0.60899999999999999</v>
+        <v>0.67859999999999987</v>
       </c>
       <c r="K19" s="2">
         <f>J19*Feuil2!$B$1</f>
-        <v>40.194000000000003</v>
+        <v>44.787599999999991</v>
       </c>
       <c r="L19" s="1">
         <v>2179</v>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="E20" s="9">
         <f t="shared" si="1"/>
-        <v>0.10218813559322035</v>
+        <v>0.11386677966101694</v>
       </c>
       <c r="F20" s="9">
         <f t="shared" si="2"/>
@@ -1806,18 +1806,18 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="H20" s="3">
-        <v>1.05</v>
+        <v>1.17</v>
       </c>
       <c r="I20">
         <v>0.57999999999999996</v>
       </c>
       <c r="J20">
         <f t="shared" ref="J20:J21" si="9">I20*H20</f>
-        <v>0.60899999999999999</v>
+        <v>0.67859999999999987</v>
       </c>
       <c r="K20" s="2">
         <f>J20*Feuil2!$B$1</f>
-        <v>40.194000000000003</v>
+        <v>44.787599999999991</v>
       </c>
       <c r="L20" s="1">
         <v>2179</v>

</xml_diff>

<commit_message>
Deer hunter as 338 Federal
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.richard\Documents\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Stalker_GAMMA\G.A.M.M.A\modpack_addons\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -236,7 +236,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +282,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -303,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -323,6 +330,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,7 +615,7 @@
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,43 +755,43 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>54</v>
+      <c r="B3" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="C3">
-        <v>6600</v>
+        <v>4000</v>
       </c>
       <c r="D3" s="4">
         <f>C3/10</f>
-        <v>660</v>
-      </c>
-      <c r="E3" s="9">
+        <v>400</v>
+      </c>
+      <c r="E3" s="14">
         <f>K3/D3</f>
-        <v>0.32129999999999992</v>
+        <v>1.500675</v>
       </c>
       <c r="F3" s="8">
         <f>G3/D3*100</f>
-        <v>2.7272727272727275E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G3">
         <v>0.18</v>
       </c>
       <c r="H3" s="3">
-        <v>3.78</v>
+        <v>10.7</v>
       </c>
       <c r="I3">
         <v>0.85</v>
       </c>
       <c r="J3">
         <f>H3*I3</f>
-        <v>3.2129999999999996</v>
+        <v>9.0949999999999989</v>
       </c>
       <c r="K3" s="2">
         <f>J3*Feuil2!$B$1</f>
-        <v>212.05799999999996</v>
+        <v>600.27</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>

</xml_diff>

<commit_message>
Slightly nerfed Hydroshock damage (64 -> 60) + slightly reduced price
</commit_message>
<xml_diff>
--- a/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
+++ b/G.A.M.M.A/modpack_addons/gamma_ammo_weapon_table.xlsx
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,7 +2799,7 @@
       </c>
       <c r="E36" s="10">
         <f t="shared" si="21"/>
-        <v>0.50239199999999995</v>
+        <v>0.47625600000000001</v>
       </c>
       <c r="F36" s="9">
         <f t="shared" si="2"/>
@@ -2809,18 +2809,18 @@
         <v>0.1</v>
       </c>
       <c r="H36" s="3">
-        <v>1.73</v>
+        <v>1.64</v>
       </c>
       <c r="I36">
         <v>0.55000000000000004</v>
       </c>
       <c r="J36">
         <f t="shared" ref="J36:J37" si="31">I36*H36</f>
-        <v>0.95150000000000001</v>
+        <v>0.90200000000000002</v>
       </c>
       <c r="K36" s="2">
         <f>J36*Feuil2!$B$1</f>
-        <v>62.798999999999999</v>
+        <v>59.532000000000004</v>
       </c>
       <c r="L36" s="1">
         <v>559</v>

</xml_diff>